<commit_message>
uploaded the visualization tool (vgps in southenr hemisphere), but works just with cartopy I guess, I tried to set the ven from the yml without success
</commit_message>
<xml_diff>
--- a/data/Poles_NAM/NAM_poles_0_130.xlsx
+++ b/data/Poles_NAM/NAM_poles_0_130.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/penokean/0000_GitHub/Young_CEED_2.0/data/Poles_NAM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\TRABAJOS\2021_YOUNG_CEED\Young_CEED_2.0\data\Poles_NAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F69C7B-0FB7-0947-BEFE-A4CE495C8958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="17340" xr2:uid="{F55FAC57-83FF-524C-B8F7-08FD345791B4}"/>
+    <workbookView xWindow="0" yWindow="765" windowWidth="28800" windowHeight="17340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -633,13 +632,13 @@
     <t>K-Ar of  ?</t>
   </si>
   <si>
-    <t>ID</t>
+    <t>pole_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1058,25 +1057,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6DBC92F-D069-B741-9DD7-5F7C979A8C84}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A66"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.83203125" style="3"/>
-    <col min="5" max="5" width="10.83203125" style="5"/>
-    <col min="6" max="7" width="10.83203125" style="3"/>
-    <col min="13" max="14" width="10.83203125" style="6"/>
-    <col min="24" max="24" width="10.83203125" style="14"/>
-    <col min="26" max="27" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="31.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.875" style="3"/>
+    <col min="5" max="5" width="10.875" style="5"/>
+    <col min="6" max="7" width="10.875" style="3"/>
+    <col min="13" max="14" width="10.875" style="6"/>
+    <col min="24" max="24" width="10.875" style="14"/>
+    <col min="26" max="27" width="10.875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>199</v>
       </c>
@@ -1159,7 +1158,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -1231,7 +1230,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -1311,7 +1310,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -1391,7 +1390,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>4</v>
       </c>
@@ -1471,7 +1470,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -1547,7 +1546,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -1627,7 +1626,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -1699,7 +1698,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -1779,7 +1778,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>9</v>
       </c>
@@ -1859,7 +1858,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>10</v>
       </c>
@@ -1931,7 +1930,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>11</v>
       </c>
@@ -2011,7 +2010,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>12</v>
       </c>
@@ -2083,7 +2082,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -2159,7 +2158,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>14</v>
       </c>
@@ -2231,7 +2230,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>15</v>
       </c>
@@ -2307,7 +2306,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>16</v>
       </c>
@@ -2379,7 +2378,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -2462,7 +2461,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -2538,7 +2537,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -2614,7 +2613,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -2690,7 +2689,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -2769,7 +2768,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -2845,7 +2844,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -2921,7 +2920,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -3001,7 +3000,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -3073,7 +3072,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -3153,7 +3152,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -3233,7 +3232,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -3309,7 +3308,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -3389,7 +3388,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>30</v>
       </c>
@@ -3468,7 +3467,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>31</v>
       </c>
@@ -3548,7 +3547,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>32</v>
       </c>
@@ -3631,7 +3630,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>33</v>
       </c>
@@ -3707,7 +3706,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>34</v>
       </c>
@@ -3783,7 +3782,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>35</v>
       </c>
@@ -3856,7 +3855,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>36</v>
       </c>
@@ -3936,7 +3935,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>37</v>
       </c>
@@ -4012,7 +4011,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>38</v>
       </c>
@@ -4089,7 +4088,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>39</v>
       </c>
@@ -4158,7 +4157,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>40</v>
       </c>
@@ -4231,7 +4230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>41</v>
       </c>
@@ -4304,7 +4303,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>42</v>
       </c>
@@ -4381,7 +4380,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <v>43</v>
       </c>
@@ -4454,7 +4453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>44</v>
       </c>
@@ -4531,7 +4530,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>45</v>
       </c>
@@ -4608,7 +4607,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>46</v>
       </c>
@@ -4691,7 +4690,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <v>47</v>
       </c>
@@ -4770,7 +4769,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <v>48</v>
       </c>
@@ -4846,7 +4845,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <v>49</v>
       </c>
@@ -4918,7 +4917,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <v>50</v>
       </c>
@@ -4994,7 +4993,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <v>51</v>
       </c>
@@ -5077,7 +5076,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <v>52</v>
       </c>
@@ -5157,7 +5156,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" s="15">
         <v>53</v>
       </c>
@@ -5237,7 +5236,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <v>54</v>
       </c>
@@ -5309,7 +5308,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <v>55</v>
       </c>
@@ -5381,7 +5380,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <v>56</v>
       </c>
@@ -5453,7 +5452,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <v>57</v>
       </c>
@@ -5525,7 +5524,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <v>58</v>
       </c>
@@ -5597,7 +5596,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" s="15">
         <v>59</v>
       </c>
@@ -5672,7 +5671,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <v>60</v>
       </c>
@@ -5747,7 +5746,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <v>61</v>
       </c>
@@ -5822,7 +5821,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <v>62</v>
       </c>
@@ -5898,7 +5897,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" s="15">
         <v>63</v>
       </c>
@@ -5978,7 +5977,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <v>64</v>
       </c>
@@ -6053,7 +6052,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66" s="15">
         <v>65</v>
       </c>

</xml_diff>